<commit_message>
completata analisi statistisca del metodo static
</commit_message>
<xml_diff>
--- a/report_metodi/risultati_Static.xlsx
+++ b/report_metodi/risultati_Static.xlsx
@@ -8,24 +8,49 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\melo\Bakarà\Counting_Bakar-\report_metodi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1399DD2-8480-46C7-AE2B-EB47BA02B8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D90D802-8A4F-4907-B4D0-50D008DA86C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Simulazione</t>
   </si>
   <si>
     <t>Bilancio_Finale</t>
+  </si>
+  <si>
+    <t>La linea gialla rappresenta la tendenza del grafico</t>
+  </si>
+  <si>
+    <t>Partite positive</t>
+  </si>
+  <si>
+    <t>Partite negative</t>
+  </si>
+  <si>
+    <t>Media</t>
   </si>
 </sst>
 </file>
@@ -81,11 +106,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -101,6 +130,1106 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="it-IT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="it-IT"/>
+              <a:t>Analisi bilancio di 50 partite</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="it-IT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4F81BD"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+            <a:scene3d>
+              <a:camera prst="orthographicFront">
+                <a:rot lat="0" lon="0" rev="0"/>
+              </a:camera>
+              <a:lightRig rig="threePt" dir="t">
+                <a:rot lat="0" lon="0" rev="1200000"/>
+              </a:lightRig>
+            </a:scene3d>
+            <a:sp3d>
+              <a:bevelT w="63500" h="25400"/>
+            </a:sp3d>
+          </c:spPr>
+          <c:invertIfNegative val="1"/>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FFFF00">
+                    <a:alpha val="97000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>-160</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-70</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-90</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-180</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-110</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-210</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-130</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-140</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-150</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{6F2FDCE9-48DA-4B69-8628-5D25D57E5C99}">
+              <c14:invertSolidFillFmt>
+                <c14:spPr xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+                  <a:solidFill>
+                    <a:srgbClr val="FF0000"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="35000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                  <a:scene3d>
+                    <a:camera prst="orthographicFront">
+                      <a:rot lat="0" lon="0" rev="0"/>
+                    </a:camera>
+                    <a:lightRig rig="threePt" dir="t">
+                      <a:rot lat="0" lon="0" rev="1200000"/>
+                    </a:lightRig>
+                  </a:scene3d>
+                  <a:sp3d>
+                    <a:bevelT w="63500" h="25400"/>
+                  </a:sp3d>
+                </c14:spPr>
+              </c14:invertSolidFillFmt>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CB04-4FFD-B8B6-759CE207C751}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="1762130463"/>
+        <c:axId val="1762130943"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1762130463"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762130943"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1762130943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="it-IT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1762130463"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="it-IT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAB51E63-21AF-A68A-DA80-16117AD6ED0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B9CD9E8-325B-41F2-9691-C06525714F67}" name="Tabella1" displayName="Tabella1" ref="O8:Q9" totalsRowShown="0">
+  <autoFilter ref="O8:Q9" xr:uid="{4B9CD9E8-325B-41F2-9691-C06525714F67}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{870BAD5E-AA96-457F-B9DF-01716D67E169}" name="Partite positive">
+      <calculatedColumnFormula>COUNTIF(B2:B51,"&gt;0")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{6F0CEE90-44AA-480A-B0B3-E3409FC47282}" name="Partite negative">
+      <calculatedColumnFormula>COUNTIF(B2:B51,"&lt;0")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{37CFB927-8864-4A48-A9FB-44E6557F80A2}" name="Media">
+      <calculatedColumnFormula>INT(AVERAGE(B2:B51))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -388,17 +1517,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" customWidth="1"/>
     <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="15" max="15" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -406,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -414,15 +1549,21 @@
         <v>-160</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>-120</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -430,7 +1571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -438,7 +1579,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -446,7 +1587,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -454,151 +1595,361 @@
         <v>-110</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O8" t="s">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9">
+        <f>COUNTIF(B2:B51,"&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="P9">
+        <f>COUNTIF(B2:B51,"&lt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="Q9">
+        <f>INT(AVERAGE(B2:B51))</f>
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>-20</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>-130</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>-70</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>-70</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>-90</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>-50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>-10</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>-20</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>-100</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -606,7 +1957,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -614,7 +1965,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -622,7 +1973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -630,7 +1981,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -638,7 +1989,7 @@
         <v>-50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -646,7 +1997,7 @@
         <v>-180</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -808,5 +2159,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>